<commit_message>
Atualização de documentos modelos de testes
</commit_message>
<xml_diff>
--- a/Documento de Testes - MODELO.xlsx
+++ b/Documento de Testes - MODELO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Arquivos\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26BE430-ECF2-456E-A841-7BB1820C4C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D9DAF5-E525-40CB-8A1C-252F21AF8E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5BE0A3A6-481A-4308-8183-1336BCDC9DDC}"/>
   </bookViews>
@@ -183,12 +183,6 @@
     <t>Ser usuário cadastrado no Spotify</t>
   </si>
   <si>
-    <t>Localizar uma música no Spotify pela seção "Pesquisar" no aplicativo desktop</t>
-  </si>
-  <si>
-    <t>o usuário tenha conta no Spotify, esteja usando o app desktop e clicou na seção "Pesquisar" do menu lateral</t>
-  </si>
-  <si>
     <t>digitar o nome de alguma música no campo de pesquisa "O que você quer ouvir?"</t>
   </si>
   <si>
@@ -202,6 +196,12 @@
   </si>
   <si>
     <t>Anexar print comprovando o resultado com data e hora</t>
+  </si>
+  <si>
+    <t>Localizar uma música no Spotify pela seção "Buscar" no site</t>
+  </si>
+  <si>
+    <t>o usuário tenha conta no Spotify, esteja usando-o no navegador e clicou na seção "Buscar" do menu lateral da tela</t>
   </si>
 </sst>
 </file>
@@ -392,6 +392,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -403,12 +409,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,27 +437,27 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>195944</xdr:colOff>
+      <xdr:colOff>174171</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>43005</xdr:rowOff>
+      <xdr:rowOff>32658</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>4321629</xdr:colOff>
+      <xdr:colOff>4310743</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>2373085</xdr:rowOff>
+      <xdr:rowOff>2363128</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
+        <xdr:cNvPr id="3" name="Imagem 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{398EF216-9B9F-1B7D-C206-F148673D585B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9061B4F4-A29B-0E15-E34D-A362E556E562}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -475,31 +475,21 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="18549258" y="957405"/>
-          <a:ext cx="4125685" cy="2330080"/>
+          <a:off x="18527485" y="947058"/>
+          <a:ext cx="4136572" cy="2330470"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -814,10 +804,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -836,10 +826,10 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -874,10 +864,10 @@
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="19"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -933,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D184ECE-7C47-4192-B519-27F7E0C35DDB}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,37 +976,37 @@
       <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" s="19" t="s">
+      <c r="J2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="15" t="s">
         <v>45</v>
       </c>
       <c r="L2" s="9"/>
@@ -1029,29 +1019,29 @@
         <v>34</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="I3" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L3" s="9"/>
     </row>

</xml_diff>